<commit_message>
add Remittance Report mPay and RabbitTopUp
</commit_message>
<xml_diff>
--- a/src/KE-PDC.Web/wwwroot/assets/templates/DailyRevenueVerifyReport.xlsx
+++ b/src/KE-PDC.Web/wwwroot/assets/templates/DailyRevenueVerifyReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ke-pdc-web-v2\ke-pdc-web-v2\src\KE-PDC.Web\wwwroot\assets\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15EF8C14-F1DD-499D-8837-DB3ED80BB933}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786011B9-D850-4A4B-90C5-201447B9B5E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-4755" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily Revenue Verify" sheetId="1" r:id="rId1"/>
@@ -623,16 +623,28 @@
     <xf numFmtId="164" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="9" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="9" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="9" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="165" fontId="3" fillId="9" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="9" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="10" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -665,23 +677,11 @@
     <xf numFmtId="0" fontId="3" fillId="18" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="9" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="9" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="9" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="10" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1091,8 +1091,8 @@
     <col min="13" max="13" width="12" style="4" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.5703125" style="56" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.28515625" style="56" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.5703125" style="38" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.28515625" style="38" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10" style="4" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="10.42578125" style="25" bestFit="1" customWidth="1"/>
@@ -1117,229 +1117,229 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" s="16" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A1" s="41"/>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="43" t="s">
+      <c r="A1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
-      <c r="P1" s="43"/>
-      <c r="Q1" s="43"/>
-      <c r="R1" s="43"/>
-      <c r="S1" s="43"/>
-      <c r="T1" s="43"/>
-      <c r="U1" s="43"/>
-      <c r="V1" s="43"/>
-      <c r="W1" s="43"/>
-      <c r="X1" s="43"/>
-      <c r="Y1" s="43"/>
-      <c r="Z1" s="43"/>
-      <c r="AA1" s="43"/>
-      <c r="AB1" s="43"/>
-      <c r="AC1" s="43"/>
-      <c r="AD1" s="43"/>
-      <c r="AE1" s="43"/>
-      <c r="AF1" s="43"/>
-      <c r="AG1" s="43"/>
-      <c r="AH1" s="43"/>
-      <c r="AI1" s="43"/>
-      <c r="AJ1" s="43"/>
-      <c r="AK1" s="43"/>
-      <c r="AL1" s="43"/>
-      <c r="AM1" s="43"/>
-      <c r="AN1" s="43"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="47"/>
+      <c r="AD1" s="47"/>
+      <c r="AE1" s="47"/>
+      <c r="AF1" s="47"/>
+      <c r="AG1" s="47"/>
+      <c r="AH1" s="47"/>
+      <c r="AI1" s="47"/>
+      <c r="AJ1" s="47"/>
+      <c r="AK1" s="47"/>
+      <c r="AL1" s="47"/>
+      <c r="AM1" s="47"/>
+      <c r="AN1" s="47"/>
       <c r="AO1" s="31"/>
     </row>
     <row r="2" spans="1:41" s="17" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="A2" s="42"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="44" t="s">
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="44"/>
-      <c r="S2" s="44"/>
-      <c r="T2" s="44"/>
-      <c r="U2" s="44"/>
-      <c r="V2" s="44"/>
-      <c r="W2" s="44"/>
-      <c r="X2" s="44"/>
-      <c r="Y2" s="44"/>
-      <c r="Z2" s="44"/>
-      <c r="AA2" s="44"/>
-      <c r="AB2" s="44"/>
-      <c r="AC2" s="44"/>
-      <c r="AD2" s="44"/>
-      <c r="AE2" s="44"/>
-      <c r="AF2" s="44"/>
-      <c r="AG2" s="44"/>
-      <c r="AH2" s="44"/>
-      <c r="AI2" s="44"/>
-      <c r="AJ2" s="44"/>
-      <c r="AK2" s="44"/>
-      <c r="AL2" s="44"/>
-      <c r="AM2" s="44"/>
-      <c r="AN2" s="44"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="48"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="48"/>
+      <c r="U2" s="48"/>
+      <c r="V2" s="48"/>
+      <c r="W2" s="48"/>
+      <c r="X2" s="48"/>
+      <c r="Y2" s="48"/>
+      <c r="Z2" s="48"/>
+      <c r="AA2" s="48"/>
+      <c r="AB2" s="48"/>
+      <c r="AC2" s="48"/>
+      <c r="AD2" s="48"/>
+      <c r="AE2" s="48"/>
+      <c r="AF2" s="48"/>
+      <c r="AG2" s="48"/>
+      <c r="AH2" s="48"/>
+      <c r="AI2" s="48"/>
+      <c r="AJ2" s="48"/>
+      <c r="AK2" s="48"/>
+      <c r="AL2" s="48"/>
+      <c r="AM2" s="48"/>
+      <c r="AN2" s="48"/>
       <c r="AO2" s="32"/>
     </row>
     <row r="3" spans="1:41" s="13" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="37" t="s">
+      <c r="E3" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="37" t="s">
+      <c r="F3" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="37" t="s">
+      <c r="G3" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="37" t="s">
+      <c r="H3" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="37" t="s">
+      <c r="I3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="37" t="s">
+      <c r="J3" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="37" t="s">
+      <c r="K3" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="37" t="s">
+      <c r="L3" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="M3" s="37" t="s">
+      <c r="M3" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="37" t="s">
+      <c r="N3" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="37" t="s">
+      <c r="O3" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="37" t="s">
+      <c r="P3" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="37" t="s">
+      <c r="Q3" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="R3" s="37" t="s">
+      <c r="R3" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="S3" s="37" t="s">
+      <c r="S3" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="T3" s="51" t="s">
+      <c r="T3" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="U3" s="53"/>
-      <c r="V3" s="37" t="s">
+      <c r="U3" s="41"/>
+      <c r="V3" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="W3" s="37" t="s">
+      <c r="W3" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="X3" s="37" t="s">
+      <c r="X3" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="Y3" s="37" t="s">
+      <c r="Y3" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="Z3" s="37" t="s">
+      <c r="Z3" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="AA3" s="37" t="s">
+      <c r="AA3" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="AB3" s="37" t="s">
+      <c r="AB3" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="AC3" s="54" t="s">
+      <c r="AC3" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="AD3" s="54"/>
-      <c r="AE3" s="54"/>
-      <c r="AF3" s="54"/>
-      <c r="AG3" s="54"/>
-      <c r="AH3" s="54"/>
-      <c r="AI3" s="54"/>
-      <c r="AJ3" s="54"/>
-      <c r="AK3" s="54"/>
-      <c r="AL3" s="51" t="s">
+      <c r="AD3" s="44"/>
+      <c r="AE3" s="44"/>
+      <c r="AF3" s="44"/>
+      <c r="AG3" s="44"/>
+      <c r="AH3" s="44"/>
+      <c r="AI3" s="44"/>
+      <c r="AJ3" s="44"/>
+      <c r="AK3" s="44"/>
+      <c r="AL3" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="AM3" s="52"/>
-      <c r="AN3" s="52"/>
-      <c r="AO3" s="53"/>
+      <c r="AM3" s="40"/>
+      <c r="AN3" s="40"/>
+      <c r="AO3" s="41"/>
     </row>
     <row r="4" spans="1:41" s="15" customFormat="1" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A4" s="50"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
-      <c r="N4" s="38"/>
-      <c r="O4" s="38"/>
-      <c r="P4" s="38"/>
-      <c r="Q4" s="38"/>
-      <c r="R4" s="38"/>
-      <c r="S4" s="38"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="43"/>
+      <c r="Q4" s="43"/>
+      <c r="R4" s="43"/>
+      <c r="S4" s="43"/>
       <c r="T4" s="26" t="s">
         <v>31</v>
       </c>
       <c r="U4" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="V4" s="38"/>
-      <c r="W4" s="38"/>
-      <c r="X4" s="38"/>
-      <c r="Y4" s="38"/>
-      <c r="Z4" s="38"/>
-      <c r="AA4" s="38"/>
-      <c r="AB4" s="38"/>
+      <c r="V4" s="43"/>
+      <c r="W4" s="43"/>
+      <c r="X4" s="43"/>
+      <c r="Y4" s="43"/>
+      <c r="Z4" s="43"/>
+      <c r="AA4" s="43"/>
+      <c r="AB4" s="43"/>
       <c r="AC4" s="18" t="s">
         <v>11</v>
       </c>
@@ -1396,8 +1396,8 @@
       <c r="M5" s="10"/>
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
-      <c r="P5" s="55"/>
-      <c r="Q5" s="55"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
       <c r="R5" s="10"/>
       <c r="S5" s="10"/>
       <c r="T5" s="24"/>
@@ -1425,17 +1425,11 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="AL3:AO3"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="AC3:AK3"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="D3:D4"/>
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="A1:D2"/>
     <mergeCell ref="W3:W4"/>
@@ -1452,11 +1446,17 @@
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="A3:A4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="AL3:AO3"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="AC3:AK3"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>